<commit_message>
Committing the changes and new file
</commit_message>
<xml_diff>
--- a/src/test/resources/com/shikha/excel/testdata.xlsx
+++ b/src/test/resources/com/shikha/excel/testdata.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14010" windowHeight="2325"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
+    <sheet name="LoginTest" sheetId="4" r:id="rId2"/>
+    <sheet name="EditAccountTest" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -21,34 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
-  <si>
-    <t>A234wd</t>
-  </si>
-  <si>
-    <t>alerttext</t>
-  </si>
-  <si>
-    <t>Customer added successfully</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>Rupee</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>TCID</t>
   </si>
@@ -56,46 +29,28 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>BankManagerLoginTest</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>AddCustomerTest</t>
-  </si>
-  <si>
-    <t>OpenAccountTest</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>runmode</t>
-  </si>
-  <si>
-    <t>Shikha</t>
-  </si>
-  <si>
-    <t>Sadana</t>
-  </si>
-  <si>
-    <t>Chetan</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>teatsdfs</t>
-  </si>
-  <si>
-    <t>atdfs</t>
-  </si>
-  <si>
-    <t>sdfdg</t>
-  </si>
-  <si>
-    <t>Shikha Sadana</t>
+    <t>LoginTest</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>shikhakumari904@gmail.com</t>
+  </si>
+  <si>
+    <t>shikha@4190</t>
+  </si>
+  <si>
+    <t>EditAccountTest</t>
   </si>
 </sst>
 </file>
@@ -413,44 +368,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -460,97 +407,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -560,31 +444,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>